<commit_message>
Final updated version of appendix tables
</commit_message>
<xml_diff>
--- a/tables/Appendix Table S1_+Spores_TP_SEM_output.xlsx
+++ b/tables/Appendix Table S1_+Spores_TP_SEM_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlfea\OneDrive\Documents\PROJECTS\Rachel Bag Experiment SEM\Data and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/Rachel Bag Experiment SEM/Data and Code/nutrient-bag-expt/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DD4396-0B1C-4FB5-8F80-5AF9AEBFCAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{30DD4396-0B1C-4FB5-8F80-5AF9AEBFCAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAE80348-1BED-44A1-A8DD-78E8B168FDE8}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="6885" windowWidth="29040" windowHeight="15840" xr2:uid="{45B3C3C3-E525-4F33-8866-CCD620B1EB35}"/>
+    <workbookView xWindow="30825" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{45B3C3C3-E525-4F33-8866-CCD620B1EB35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Estimate</t>
   </si>
@@ -84,9 +84,6 @@
     </r>
   </si>
   <si>
-    <t>Infection Density</t>
-  </si>
-  <si>
     <t>Total Host Density</t>
   </si>
   <si>
@@ -112,13 +109,16 @@
   <si>
     <t>&lt;0.001</t>
   </si>
+  <si>
+    <t>Infected Host Density</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -249,15 +249,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -275,72 +279,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDB78186-ECFD-4AB6-98B8-3CAE3093842B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8553450" y="590550"/>
-          <a:ext cx="6619875" cy="1666875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -640,260 +578,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B409768-71E1-416A-BBC7-5D838A948E2F}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="B3" sqref="B3:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+    <row r="4" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D4" s="12">
+        <v>7.8982350753962705E-2</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.45745510538470302</v>
+      </c>
+      <c r="F4" s="13">
+        <v>9.9140365532747205E-3</v>
+      </c>
+      <c r="G4">
+        <v>79</v>
+      </c>
+      <c r="H4" s="13">
+        <v>7.9667197442270901</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12">
-        <v>8.3497960656471804E-2</v>
-      </c>
-      <c r="D2" s="12">
-        <v>0.48507912294713001</v>
-      </c>
-      <c r="E2" s="13">
-        <v>9.8727951142912902E-3</v>
-      </c>
-      <c r="F2">
+      <c r="D5" s="13">
+        <v>4.9578028620363E-2</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1.9068226633687499E-2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.131706837922107</v>
+      </c>
+      <c r="G5" s="9">
         <v>79</v>
       </c>
-      <c r="G2" s="13">
-        <v>8.45737804642628</v>
-      </c>
-      <c r="H2" s="17" t="s">
+      <c r="H5" s="13">
+        <v>0.37642714229981</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0.70659937071019396</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-1.0192759503156399E-2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>-0.106974872050989</v>
+      </c>
+      <c r="F6" s="14">
+        <v>6.2842243623436296E-3</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="14">
+        <v>-1.62195983393488</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.104811948645847</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="18">
+        <v>-1.27491670389777E-2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>-0.232070005783066</v>
+      </c>
+      <c r="F7" s="18">
+        <v>8.6461318366876996E-3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>79</v>
+      </c>
+      <c r="H7" s="18">
+        <v>-1.47455154279279</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0.14033315076103201</v>
+      </c>
+      <c r="K7">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.331837421777398</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.221357180783675</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.228449360502055</v>
+      </c>
+      <c r="G8" s="6">
+        <v>79</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1.45256445913497</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.146344719964285</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="12">
+        <v>5.2955636732877703E-2</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.25838299509866502</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1.4073480017322599E-2</v>
+      </c>
+      <c r="G9">
+        <v>79</v>
+      </c>
+      <c r="H9" s="13">
+        <v>3.76279617178526</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+      <c r="K9">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="14">
+        <v>8.0792630248927202E-2</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4.3394396107672997E-2</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.41939093146596701</v>
+      </c>
+      <c r="G10" s="6">
+        <v>79</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.19264276880408299</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.84723874758505802</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="14">
-        <v>5.8076766088417997E-2</v>
-      </c>
-      <c r="D3" s="14">
-        <v>2.2404835955921201E-2</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0.14194733241108201</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="C11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.15046546646277301</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0.15046546646277301</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="8">
         <v>79</v>
       </c>
-      <c r="G3" s="14">
-        <v>0.40914306103496501</v>
-      </c>
-      <c r="H3" s="14">
-        <v>0.68243467690809101</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="13">
-        <v>-1.2749169609843101E-2</v>
-      </c>
-      <c r="D4" s="13">
-        <v>-0.23207001714213499</v>
-      </c>
-      <c r="E4" s="13">
-        <v>8.6461354776976602E-3</v>
-      </c>
-      <c r="F4">
-        <v>79</v>
-      </c>
-      <c r="G4" s="13">
-        <v>-1.47455121918099</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.14033323782145601</v>
-      </c>
-      <c r="J4">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.33183652470745301</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.22135654857777901</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0.22844971660744101</v>
-      </c>
-      <c r="F5" s="6">
-        <v>79</v>
-      </c>
-      <c r="G5" s="14">
-        <v>1.4525582681184399</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0.14634643999248201</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="12">
-        <v>5.2955633944812501E-2</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.258382980300362</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1.4073479731131201E-2</v>
-      </c>
-      <c r="F6">
-        <v>79</v>
-      </c>
-      <c r="G6" s="13">
-        <v>3.7627960501958801</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="15">
-        <v>8.0792633258755797E-2</v>
-      </c>
-      <c r="D7" s="15">
-        <v>4.3394397523635601E-2</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0.419391147263873</v>
-      </c>
-      <c r="F7" s="9">
-        <v>79</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0.19264267685632</v>
-      </c>
-      <c r="H7" s="15">
-        <v>0.84723881960000202</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="16">
-        <v>0.15046557280629</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0.15046557280629</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="10">
-        <v>79</v>
-      </c>
-      <c r="G8" s="16">
-        <v>1.32683412829119</v>
-      </c>
-      <c r="H8" s="16">
-        <v>9.4268193986010801E-2</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+      <c r="H11" s="19">
+        <v>1.32683316881127</v>
+      </c>
+      <c r="I11" s="19">
+        <v>9.4268351972580905E-2</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>